<commit_message>
Added  "Power On" led and updated design files
Added  "Power On" led and updated design files
</commit_message>
<xml_diff>
--- a/hardware/doc/druino_uno_bom.xlsx
+++ b/hardware/doc/druino_uno_bom.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Altium\druino-uno\hardware\altium_source\Project Outputs for druino_uno\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{809CC9CC-9509-44F1-A352-6D8299C5E304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD46981C-1F7C-474E-B232-92B7006101FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28695" yWindow="3120" windowWidth="28800" windowHeight="11295" xr2:uid="{98332964-E8AE-4C32-B035-0EC00C42544F}"/>
+    <workbookView xWindow="180" yWindow="3435" windowWidth="28800" windowHeight="11295" xr2:uid="{B8BCBBC8-4DF8-4626-BFC6-9556CF4A93ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="druino_uno_bom" sheetId="1" r:id="rId1"/>
+    <sheet name="druino_uno" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">druino_uno_bom!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">druino_uno!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,22 +30,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="180">
   <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Designator</t>
+  </si>
+  <si>
     <t>Comment</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Designator</t>
-  </si>
-  <si>
-    <t>Quantity</t>
+    <t>Part Number</t>
   </si>
   <si>
     <t>Manufacturer</t>
   </si>
   <si>
-    <t>Part Number</t>
+    <t>A1</t>
   </si>
   <si>
     <t>ESP32-S3-MINI-1-N8</t>
@@ -54,118 +57,118 @@
     <t>2.4 GHz WiFi + Bluetooth® + Bluetooth LE module</t>
   </si>
   <si>
-    <t>A1</t>
-  </si>
-  <si>
     <t>Espressif Systems</t>
   </si>
   <si>
+    <t>C1, C2, C4, C5, C6, C8, C12, C19, C23, C24, C25</t>
+  </si>
+  <si>
     <t>0.1u</t>
   </si>
   <si>
     <t>Capacitors 0402 package case</t>
   </si>
   <si>
-    <t>C1, C2, C4, C5, C6, C8, C12, C19, C23, C24, C25</t>
+    <t>TCC0402X7R104J500AT</t>
   </si>
   <si>
     <t>CCTC</t>
   </si>
   <si>
-    <t>TCC0402X7R104J500AT</t>
+    <t>C3, C7, C9, C10, C20</t>
   </si>
   <si>
     <t>12p</t>
   </si>
   <si>
-    <t>C3, C7, C9, C10, C20</t>
-  </si>
-  <si>
     <t>TCC0402COG120F500AT</t>
   </si>
   <si>
+    <t>C11</t>
+  </si>
+  <si>
     <t>1u</t>
   </si>
   <si>
     <t>Capacitors 0603 package case</t>
   </si>
   <si>
-    <t>C11</t>
-  </si>
-  <si>
     <t>TCC0603X7R106M6R3CT</t>
   </si>
   <si>
+    <t>C13, C14</t>
+  </si>
+  <si>
     <t>0.047u</t>
   </si>
   <si>
-    <t>C13, C14</t>
-  </si>
-  <si>
     <t>TCC0603X7R473K500CT</t>
   </si>
   <si>
+    <t>C15</t>
+  </si>
+  <si>
     <t>2200p</t>
   </si>
   <si>
     <t>Capacitors 1206 package case</t>
   </si>
   <si>
-    <t>C15</t>
-  </si>
-  <si>
     <t>TCC1206X7R222K102FT</t>
   </si>
   <si>
+    <t>C16</t>
+  </si>
+  <si>
     <t>4700p</t>
   </si>
   <si>
-    <t>C16</t>
-  </si>
-  <si>
     <t>TCC1206X7R472K102FT</t>
   </si>
   <si>
+    <t>C17, C18</t>
+  </si>
+  <si>
     <t>10u</t>
   </si>
   <si>
     <t>Capacitors 0805 package case</t>
   </si>
   <si>
-    <t>C17, C18</t>
-  </si>
-  <si>
     <t>TCC0805X7R106K250FT</t>
   </si>
   <si>
+    <t>C21, C22</t>
+  </si>
+  <si>
     <t>22u</t>
   </si>
   <si>
-    <t>C21, C22</t>
-  </si>
-  <si>
     <t>TCC1206X7R226M160HT</t>
   </si>
   <si>
+    <t>DA1</t>
+  </si>
+  <si>
     <t>TPD4E1U06DCKR</t>
   </si>
   <si>
     <t>6 Quad-Channel, High-Speed ESD Protection Device</t>
   </si>
   <si>
-    <t>DA1</t>
-  </si>
-  <si>
     <t>Texas Instruments</t>
   </si>
   <si>
+    <t>DA2</t>
+  </si>
+  <si>
     <t>TPS63060DSC</t>
   </si>
   <si>
     <t>High Input Voltage, 2A Buck-Boost Converter</t>
   </si>
   <si>
-    <t>DA2</t>
+    <t>DA3</t>
   </si>
   <si>
     <t>PRTR5V0U2X</t>
@@ -174,31 +177,31 @@
     <t>Ultra low capacitance double rail-to-rail ESD protection diode</t>
   </si>
   <si>
-    <t>DA3</t>
-  </si>
-  <si>
     <t>NXP USA Inc.</t>
   </si>
   <si>
+    <t>DD1</t>
+  </si>
+  <si>
     <t>CH32V307RCT6</t>
   </si>
   <si>
     <t>RISC-V MCU 144MHz with 256KB flash, 64KB RAM</t>
   </si>
   <si>
-    <t>DD1</t>
-  </si>
-  <si>
     <t>WinChipHead</t>
   </si>
   <si>
+    <t>DD2</t>
+  </si>
+  <si>
     <t>CH549G</t>
   </si>
   <si>
     <t>8-bit Enhanced USB MCU</t>
   </si>
   <si>
-    <t>DD2</t>
+    <t>DD3</t>
   </si>
   <si>
     <t>CH442E</t>
@@ -207,7 +210,7 @@
     <t>Double-pole Double-throw Low-Resistance Analog Switch IC</t>
   </si>
   <si>
-    <t>DD3</t>
+    <t>HL1, HL2, HL3, HL4, HL5</t>
   </si>
   <si>
     <t>KPHHS-1005ZGC-V</t>
@@ -216,19 +219,19 @@
     <t>Green led (package case 0402)</t>
   </si>
   <si>
-    <t>HL1, HL2, HL3, HL4</t>
-  </si>
-  <si>
     <t>Kingbright Company LLC.</t>
   </si>
   <si>
+    <t>HL6</t>
+  </si>
+  <si>
     <t>KPHHS-1005SURCK</t>
   </si>
   <si>
     <t>Red led (package case 0402)</t>
   </si>
   <si>
-    <t>HL5</t>
+    <t>HL7, HL8, HL9, HL10, HL11, HL12, HL13, HL14, HL15, HL16, HL17, HL18, HL19, HL20, HL21, HL22, HL23, HL24, HL25, HL26, HL27, HL28, HL29, HL30, HL31, HL32, HL33, HL34, HL35, HL36, HL37, HL38, HL39, HL40, HL41, HL42, HL43, HL44, HL45, HL46, HL47, HL48, HL49, HL50, HL51, HL52, HL53, HL54, HL55, HL56, HL57, HL58, HL59, HL60, HL61, HL62, HL63, HL64, HL65, HL66, HL67, HL68, HL69, HL70, HL71, HL72, HL73, HL74, HL75, HL76, HL77, HL78, HL79, HL80, HL81, HL82, HL83, HL84, HL85, HL86, HL87, HL88, HL89, HL90, HL91, HL92, HL93, HL94, HL95, HL96, HL97, HL98, HL99, HL100, HL101, HL102, HL103</t>
   </si>
   <si>
     <t>KPHHS-1005QBC-D-V</t>
@@ -237,7 +240,7 @@
     <t>Blue led (package case 0402)</t>
   </si>
   <si>
-    <t>HL6, HL7, HL8, HL9, HL10, HL11, HL12, HL13, HL14, HL15, HL16, HL17, HL18, HL19, HL20, HL21, HL22, HL23, HL24, HL25, HL26, HL27, HL28, HL29, HL30, HL31, HL32, HL33, HL34, HL35, HL36, HL37, HL38, HL39, HL40, HL41, HL42, HL43, HL44, HL45, HL46, HL47, HL48, HL49, HL50, HL51, HL52, HL53, HL54, HL55, HL56, HL57, HL58, HL59, HL60, HL61, HL62, HL63, HL64, HL65, HL66, HL67, HL68, HL69, HL70, HL71, HL72, HL73, HL74, HL75, HL76, HL77, HL78, HL79, HL80, HL81, HL82, HL83, HL84, HL85, HL86, HL87, HL88, HL89, HL90, HL91, HL92, HL93, HL94, HL95, HL96, HL97, HL98, HL99, HL100, HL101, HL102</t>
+    <t>L1</t>
   </si>
   <si>
     <t>IHLP2020BZERR22M01</t>
@@ -246,96 +249,93 @@
     <t>Shielded SMD Power Inductors</t>
   </si>
   <si>
-    <t>L1</t>
-  </si>
-  <si>
     <t>Vishay Dale</t>
   </si>
   <si>
+    <t>R1, R29, R33</t>
+  </si>
+  <si>
     <t>10k</t>
   </si>
   <si>
     <t>Resistor 0402 package case</t>
   </si>
   <si>
-    <t>R1, R29, R32</t>
+    <t>RC0402FR-0710KL</t>
   </si>
   <si>
     <t>Yageo</t>
   </si>
   <si>
-    <t>RC0402FR-0710KL</t>
+    <t>R2, R12, R13, R14</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>R2, R12, R13, R14</t>
-  </si>
-  <si>
     <t>RC0402FR-070RL</t>
   </si>
   <si>
+    <t>R3, R5, R6, R7</t>
+  </si>
+  <si>
     <t>4.7k</t>
   </si>
   <si>
-    <t>R3, R5, R6, R7</t>
-  </si>
-  <si>
     <t>RC0402FR-074K7L</t>
   </si>
   <si>
+    <t>R4</t>
+  </si>
+  <si>
     <t>Resistor 0603 package case</t>
   </si>
   <si>
-    <t>R4</t>
-  </si>
-  <si>
     <t>RC0603FR-074K7L</t>
   </si>
   <si>
+    <t>R8, R9, R10, R11, R32, R35</t>
+  </si>
+  <si>
     <t>560</t>
   </si>
   <si>
-    <t>R8, R9, R10, R11, R34</t>
-  </si>
-  <si>
     <t>RC0402FR-07560RL</t>
   </si>
   <si>
+    <t>R15, R16, R17, R30</t>
+  </si>
+  <si>
     <t>100k</t>
   </si>
   <si>
-    <t>R15, R16, R17, R30</t>
-  </si>
-  <si>
     <t>RC0402FR-07100KL</t>
   </si>
   <si>
+    <t>R18, R19, R20, R21</t>
+  </si>
+  <si>
     <t>51</t>
   </si>
   <si>
-    <t>R18, R19, R20, R21</t>
-  </si>
-  <si>
     <t>RC0603FR-0751RL</t>
   </si>
   <si>
+    <t>R22, R23, R24, R25</t>
+  </si>
+  <si>
     <t>75</t>
   </si>
   <si>
-    <t>R22, R23, R24, R25</t>
-  </si>
-  <si>
     <t>RC0603FR-0775RL</t>
   </si>
   <si>
+    <t>R26</t>
+  </si>
+  <si>
     <t>750</t>
   </si>
   <si>
-    <t>R26</t>
-  </si>
-  <si>
     <t>RC0603FR-07750RL</t>
   </si>
   <si>
@@ -345,88 +345,91 @@
     <t>RC0603FR-07560RL</t>
   </si>
   <si>
+    <t>R28</t>
+  </si>
+  <si>
     <t>1M</t>
   </si>
   <si>
-    <t>R28</t>
-  </si>
-  <si>
     <t>RC0603FR-071ML</t>
   </si>
   <si>
+    <t>R31</t>
+  </si>
+  <si>
     <t>18k</t>
   </si>
   <si>
-    <t>R31</t>
-  </si>
-  <si>
     <t>RC0402FR-0718KL</t>
   </si>
   <si>
-    <t>R33</t>
+    <t>R34</t>
   </si>
   <si>
     <t>RC0402FR-07750RL</t>
   </si>
   <si>
+    <t>R36, R37, R38, R39, R40, R41, R42, R43, R44, R45, R46</t>
+  </si>
+  <si>
     <t>330</t>
   </si>
   <si>
-    <t>R35, R36, R37, R38, R39, R40, R41, R42, R43, R44, R45</t>
-  </si>
-  <si>
     <t>RC0402FR-07330RL</t>
   </si>
   <si>
+    <t>SB1, SB2</t>
+  </si>
+  <si>
     <t>KLS7-TS3401- 2.5-180</t>
   </si>
   <si>
     <t>Tact Button SMD 4х3х2.5mm</t>
   </si>
   <si>
-    <t>SB1, SB2</t>
-  </si>
-  <si>
     <t>KLS</t>
   </si>
   <si>
+    <t>T1</t>
+  </si>
+  <si>
     <t>H1102NL</t>
   </si>
   <si>
     <t>10/100BASE-T Ethernet transformer Ratio 1:1 350 uH</t>
   </si>
   <si>
-    <t>T1</t>
-  </si>
-  <si>
     <t>Pulse Electronics</t>
   </si>
   <si>
+    <t>VD1, VD2, VD4, VD5, VD6, VD7, VD9, VD11</t>
+  </si>
+  <si>
     <t>BAS70-04</t>
   </si>
   <si>
     <t>Small Signal Schottky Diodes</t>
   </si>
   <si>
-    <t>VD1, VD2, VD4, VD5, VD6, VD7, VD9, VD11</t>
-  </si>
-  <si>
     <t>Diodes Incorporated</t>
   </si>
   <si>
+    <t>VD3, VD10</t>
+  </si>
+  <si>
     <t>BAS516,115</t>
   </si>
   <si>
     <t>High-speed switching diode</t>
   </si>
   <si>
-    <t>VD3, VD10</t>
+    <t>VD8</t>
   </si>
   <si>
     <t>BAS70-05</t>
   </si>
   <si>
-    <t>VD8</t>
+    <t>VD12, VD13</t>
   </si>
   <si>
     <t>SS34F</t>
@@ -435,28 +438,28 @@
     <t>3A Schottky barrier rectifier</t>
   </si>
   <si>
-    <t>VD12, VD13</t>
-  </si>
-  <si>
     <t>UMW</t>
   </si>
   <si>
+    <t>XP1</t>
+  </si>
+  <si>
     <t>PLD-6</t>
   </si>
   <si>
-    <t>XP1</t>
+    <t>XP2</t>
   </si>
   <si>
     <t>PLS3</t>
   </si>
   <si>
-    <t>XP2</t>
+    <t>XP3</t>
   </si>
   <si>
     <t>PLS2</t>
   </si>
   <si>
-    <t>XP3</t>
+    <t>XS1, XS4</t>
   </si>
   <si>
     <t>DS1023-1x8S21</t>
@@ -465,22 +468,22 @@
     <t>2.54mm Female Header V/T Type, H = 8.5mm</t>
   </si>
   <si>
-    <t>XS1, XS4</t>
-  </si>
-  <si>
     <t>Connfly</t>
   </si>
   <si>
+    <t>XS2</t>
+  </si>
+  <si>
     <t>DS1023-1x6S21</t>
   </si>
   <si>
-    <t>XS2</t>
+    <t>XS3</t>
   </si>
   <si>
     <t>DS1023-1x10S21</t>
   </si>
   <si>
-    <t>XS3</t>
+    <t>XS5</t>
   </si>
   <si>
     <t>SM04B-SRSS-TB(LF)(SN)</t>
@@ -489,19 +492,19 @@
     <t>CONNECTOR, HEADER, SMT, R/A, 1MM, 4WAY</t>
   </si>
   <si>
-    <t>XS5</t>
-  </si>
-  <si>
     <t>JST</t>
   </si>
   <si>
+    <t>XS6</t>
+  </si>
+  <si>
     <t>KLS12-108-8P8C-1X1-2-R/G-0-01</t>
   </si>
   <si>
     <t>RJ-45</t>
   </si>
   <si>
-    <t>XS6</t>
+    <t>XS7</t>
   </si>
   <si>
     <t>DC-042C-Z-2.0</t>
@@ -510,31 +513,31 @@
     <t>Shrouded DC Power Receptacle 2mm 6.3mm 8A 24V</t>
   </si>
   <si>
-    <t>XS7</t>
-  </si>
-  <si>
     <t>XKB Connectivity</t>
   </si>
   <si>
+    <t>XS8</t>
+  </si>
+  <si>
     <t>GT-USB-7010ASV</t>
   </si>
   <si>
     <t>USB 2.0 Female 3A Surface 16P</t>
   </si>
   <si>
-    <t>XS8</t>
-  </si>
-  <si>
     <t>G-Switch</t>
   </si>
   <si>
+    <t>Z1</t>
+  </si>
+  <si>
     <t>BLM15PX601SN1D</t>
   </si>
   <si>
     <t>Power line filter, imperdance 600 Ohm @ 100 MHz (current 0.9A)</t>
   </si>
   <si>
-    <t>Z1</t>
+    <t>Z2</t>
   </si>
   <si>
     <t>BLM18HE152SN1D</t>
@@ -543,31 +546,28 @@
     <t>Power line filter, imperdance 1500 Ohm @100MHz (current 0.5A)</t>
   </si>
   <si>
-    <t>Z2</t>
-  </si>
-  <si>
     <t>Murata</t>
   </si>
   <si>
+    <t>ZQ1</t>
+  </si>
+  <si>
     <t>X32258MOB4SI</t>
   </si>
   <si>
     <t>Quartz Crystal 8 MHz</t>
   </si>
   <si>
-    <t>ZQ1</t>
-  </si>
-  <si>
     <t>YXC</t>
   </si>
   <si>
+    <t>ZQ2</t>
+  </si>
+  <si>
     <t>X321532768KGD2SI</t>
   </si>
   <si>
     <t>Quartz Crystal 32768 Hz</t>
-  </si>
-  <si>
-    <t>ZQ2</t>
   </si>
 </sst>
 </file>
@@ -943,7 +943,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B984F764-86E1-4902-A9A7-A64C218C1032}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC9F784-3D80-4312-97C3-817AC50ADDA5}">
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -975,37 +975,37 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="1">
-        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>13</v>
@@ -1015,357 +1015,357 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1">
-        <v>5</v>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="1">
-        <v>2</v>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1">
-        <v>1</v>
+      <c r="D8" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>2</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="1">
-        <v>2</v>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
       <c r="E11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
       <c r="E12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
       <c r="E13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
       <c r="E14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
       <c r="E15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
       <c r="E16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1">
+        <v>5</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="1">
-        <v>4</v>
-      </c>
       <c r="E17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
       <c r="E18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1">
+        <v>97</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="1">
-        <v>97</v>
-      </c>
       <c r="E19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
       <c r="E20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="D21" s="1">
-        <v>3</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>77</v>
@@ -1375,643 +1375,643 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1">
+        <v>4</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>4</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="1">
-        <v>4</v>
+      <c r="D23" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>82</v>
+      <c r="A24" s="1">
+        <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="1">
-        <v>1</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="1">
-        <v>5</v>
+      <c r="D25" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1">
+        <v>4</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>4</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>4</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="1">
-        <v>4</v>
+      <c r="D28" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D29" s="1">
-        <v>1</v>
+      <c r="D29" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>88</v>
+      <c r="A30" s="1">
+        <v>1</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1</v>
+        <v>89</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1">
+        <v>1</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D31" s="1">
-        <v>1</v>
+      <c r="D31" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D32" s="1">
-        <v>1</v>
+      <c r="D32" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>100</v>
+      <c r="A33" s="1">
+        <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="1">
+        <v>11</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D34" s="1">
-        <v>11</v>
+      <c r="D34" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>77</v>
+        <v>115</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1">
+        <v>2</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D35" s="1">
+      <c r="E35" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>1</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>8</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>2</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D36" s="1">
-        <v>1</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D37" s="1">
-        <v>8</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D38" s="1">
-        <v>2</v>
-      </c>
       <c r="E38" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>128</v>
-      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1">
+        <v>1</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D39" s="1">
-        <v>1</v>
+      <c r="D39" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>131</v>
-      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1">
+        <v>2</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D40" s="1">
-        <v>2</v>
-      </c>
       <c r="E40" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>133</v>
-      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1">
+        <v>1</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B41" s="1"/>
       <c r="C41" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D41" s="1">
-        <v>1</v>
-      </c>
+      <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="1">
+        <v>1</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B42" s="1"/>
       <c r="C42" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D42" s="1">
-        <v>1</v>
-      </c>
+      <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1">
+        <v>1</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B43" s="1"/>
       <c r="C43" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D43" s="1">
-        <v>1</v>
-      </c>
+      <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="1">
+        <v>2</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D44" s="1">
-        <v>2</v>
-      </c>
       <c r="E44" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1">
+        <v>1</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D45" s="1">
-        <v>1</v>
+      <c r="D45" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="E45" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1">
+        <v>1</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D46" s="1">
-        <v>1</v>
+      <c r="D46" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="E46" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>149</v>
-      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1">
+        <v>1</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
       <c r="E47" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>151</v>
-      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1">
+        <v>1</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D48" s="1">
-        <v>1</v>
-      </c>
       <c r="E48" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F48" s="2" t="s">
-        <v>155</v>
-      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1">
+        <v>1</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D49" s="1">
-        <v>1</v>
-      </c>
       <c r="E49" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F49" s="2" t="s">
-        <v>158</v>
-      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1">
+        <v>1</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D50" s="1">
-        <v>1</v>
-      </c>
       <c r="E50" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F50" s="2" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1">
+        <v>1</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D51" s="1">
-        <v>1</v>
-      </c>
-      <c r="E51" s="1"/>
-      <c r="F51" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="E51" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1">
+        <v>1</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D52" s="1">
-        <v>1</v>
-      </c>
       <c r="E52" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F52" s="2" t="s">
-        <v>169</v>
-      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1">
+        <v>1</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D53" s="1">
-        <v>1</v>
-      </c>
       <c r="E53" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F53" s="2" t="s">
-        <v>173</v>
-      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="1">
+        <v>1</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D54" s="1">
-        <v>1</v>
-      </c>
       <c r="E54" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed filter Z1 from size 0402 to 0603
Changed filter Z1 from size 0402 to 0603
</commit_message>
<xml_diff>
--- a/hardware/doc/druino_uno_bom.xlsx
+++ b/hardware/doc/druino_uno_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Altium\druino-uno\hardware\altium_source\Project Outputs for druino_uno\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD46981C-1F7C-474E-B232-92B7006101FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F053E12B-D8FE-4B97-B50B-926A7B4DD309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="3435" windowWidth="28800" windowHeight="11295" xr2:uid="{B8BCBBC8-4DF8-4626-BFC6-9556CF4A93ED}"/>
+    <workbookView xWindow="-28695" yWindow="3435" windowWidth="28800" windowHeight="11295" xr2:uid="{F6EA08A5-8C33-4435-80F2-3CC6E97ACAE5}"/>
   </bookViews>
   <sheets>
     <sheet name="druino_uno" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="177">
   <si>
     <t>Quantity</t>
   </si>
@@ -528,16 +528,7 @@
     <t>G-Switch</t>
   </si>
   <si>
-    <t>Z1</t>
-  </si>
-  <si>
-    <t>BLM15PX601SN1D</t>
-  </si>
-  <si>
-    <t>Power line filter, imperdance 600 Ohm @ 100 MHz (current 0.9A)</t>
-  </si>
-  <si>
-    <t>Z2</t>
+    <t>Z1, Z2</t>
   </si>
   <si>
     <t>BLM18HE152SN1D</t>
@@ -943,8 +934,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC9F784-3D80-4312-97C3-817AC50ADDA5}">
-  <dimension ref="A1:F54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B14287-695D-4A69-8888-23B3847A983C}">
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1938,7 +1929,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>166</v>
@@ -1952,26 +1943,28 @@
       <c r="E51" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F51" s="1"/>
+      <c r="F51" s="2" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>1</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="F52" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1979,39 +1972,19 @@
         <v>1</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>1</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>